<commit_message>
update submissions metadata template
</commit_message>
<xml_diff>
--- a/client/public/assets/data/Sample_metadata_template.xlsx
+++ b/client/public/assets/data/Sample_metadata_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-COMPASS/Shared Documents/Methylation/CBIIT/MethylScape_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{D2FF83EE-9751-442C-B886-D4E17C3CA571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7E73451-B6E1-4BBE-8E50-C4EE9B060FA4}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{D2FF83EE-9751-442C-B886-D4E17C3CA571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7EF0C27-5DE1-4319-AEDE-50BD0CC02499}"/>
   <bookViews>
-    <workbookView xWindow="33291" yWindow="377" windowWidth="30635" windowHeight="17452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Sheet" sheetId="1" r:id="rId1"/>
@@ -588,12 +588,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -958,6 +962,25 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.0703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.92578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.2109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -1014,7 +1037,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
@@ -1057,7 +1080,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1076,7 +1099,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1095,7 +1118,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1114,7 +1137,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1133,7 +1156,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1152,7 +1175,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1171,7 +1194,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1190,7 +1213,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1209,7 +1232,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1228,7 +1251,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1247,7 +1270,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1266,7 +1289,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1285,7 +1308,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1304,7 +1327,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1323,7 +1346,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1342,7 +1365,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1361,7 +1384,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1380,7 +1403,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1399,7 +1422,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1418,7 +1441,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1437,7 +1460,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1456,7 +1479,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1475,7 +1498,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1494,7 +1517,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1513,7 +1536,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1532,7 +1555,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1551,7 +1574,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1570,7 +1593,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1589,7 +1612,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -1608,7 +1631,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -1627,7 +1650,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -1646,7 +1669,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -1665,7 +1688,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -1684,7 +1707,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -1703,7 +1726,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -1722,7 +1745,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1741,7 +1764,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1760,7 +1783,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -1779,7 +1802,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -1798,7 +1821,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -1817,7 +1840,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1836,7 +1859,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="F50" s="4"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1855,7 +1878,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="4"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -1874,7 +1897,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -1893,7 +1916,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -1912,7 +1935,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -1931,7 +1954,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -1950,7 +1973,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="F56" s="4"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -1969,7 +1992,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="F57" s="4"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -1988,7 +2011,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="F58" s="4"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -2007,7 +2030,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="F59" s="4"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -2026,7 +2049,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="F60" s="4"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -2045,7 +2068,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="F61" s="4"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -2064,7 +2087,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="4"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -2083,7 +2106,7 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="F63" s="4"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -2102,7 +2125,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="F64" s="4"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -2121,7 +2144,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="4"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -2140,7 +2163,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="F66" s="4"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -2159,7 +2182,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="F67" s="4"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -2178,7 +2201,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="F68" s="4"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -2197,7 +2220,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="F69" s="4"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -2216,7 +2239,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="F70" s="4"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -2235,7 +2258,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -2254,7 +2277,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -2273,7 +2296,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
@@ -2292,7 +2315,7 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="F74" s="4"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -2311,7 +2334,7 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="4"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
@@ -2330,7 +2353,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="F76" s="4"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -2349,7 +2372,7 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="4"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -2368,7 +2391,7 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="4"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -2382,12 +2405,34 @@
       <c r="Q78" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QRSvtRmrXpvmPxVWFWSf9MqE5B52j+YP9F8R+866VqhRcgLYPGNRGT7+7EpQ6QR/ynBmNtt8avhNdZ+9zAwjfw==" saltValue="2id+Cw7WdA6zKoz4NAHwkg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f9a0503-38ae-4166-b431-5fccf196b5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="a29b9f1f-99aa-43bf-9dd0-188afd1cbf62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100212142D758DF054DB1EB1FDCE866558F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7ef803e44bae32d73f30e02c9aa8b5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7f9a0503-38ae-4166-b431-5fccf196b5d0" xmlns:ns3="a29b9f1f-99aa-43bf-9dd0-188afd1cbf62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36b288adc7513afff68b706ba4c3061d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2653,29 +2698,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{793EEC7E-A90F-4EB3-8A3D-589AF5957184}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f9a0503-38ae-4166-b431-5fccf196b5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="a29b9f1f-99aa-43bf-9dd0-188afd1cbf62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C3E59-CE38-4C13-8D30-0F78583A7E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7f9a0503-38ae-4166-b431-5fccf196b5d0"/>
+    <ds:schemaRef ds:uri="a29b9f1f-99aa-43bf-9dd0-188afd1cbf62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B8162D4-2DAB-46FC-82FE-87883025D2E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2695,22 +2738,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{793EEC7E-A90F-4EB3-8A3D-589AF5957184}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C3E59-CE38-4C13-8D30-0F78583A7E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="7f9a0503-38ae-4166-b431-5fccf196b5d0"/>
-    <ds:schemaRef ds:uri="a29b9f1f-99aa-43bf-9dd0-188afd1cbf62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>